<commit_message>
update 227C class list
</commit_message>
<xml_diff>
--- a/studentList_M227C.xlsx
+++ b/studentList_M227C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/int/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13295BD8-0922-5E47-9269-613EAD015E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2318B72-2BA8-CD43-9CB3-97749A633075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37240" yWindow="3080" windowWidth="22140" windowHeight="21380" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Chaorong</t>
   </si>
@@ -139,13 +139,70 @@
   </si>
   <si>
     <t>Anthony</t>
+  </si>
+  <si>
+    <t>85121744        CHEN, CHAORONG  CHAORONC@UCI.EDU        MCSB    G6      GR</t>
+  </si>
+  <si>
+    <t>15841424        DE ROBLES, GABRIELA     GDEROBLE@UCI.EDU        MCSB    G5      GR</t>
+  </si>
+  <si>
+    <t>21244597        ELDEEN, SARAH   SELDEEN@UCI.EDU MCSB    G6      GR</t>
+  </si>
+  <si>
+    <t>84549672        GAO, PEIJUN     PEIJUNG@UCI.EDU MATH    JR      GR</t>
+  </si>
+  <si>
+    <t>25167480        GUERRERO RAMIREZ, ANDRES FELIPE AFGUERRE@UCI.EDU        MCSB    G6      GR</t>
+  </si>
+  <si>
+    <t>18249792        IYER, VIGNESH HARIHARAN VHIYER@UCI.EDU  MATH    G5      GR</t>
+  </si>
+  <si>
+    <t>49527062        LAI, LULU       LLAI7@UCI.EDU   MCSB    G6      GR</t>
+  </si>
+  <si>
+    <t>84409046        NGUYEN, THI THU THAO    THAOTN18@UCI.EDU        MCSB    G6      GR</t>
+  </si>
+  <si>
+    <t>61007128        OLARANONT, NONTHAKORN   NOLARANO@UCI.EDU        MATH    G6      GR</t>
+  </si>
+  <si>
+    <t>41761116        RAHIMZADEH, NEGIN       NRAHIMZA@UCI.EDU        MCSB    G6      GR</t>
+  </si>
+  <si>
+    <t>13522870        RUAN, YIBIAO    YIBIAOR@UCI.EDU MATH    G5      GR</t>
+  </si>
+  <si>
+    <t>90727596        SHAO, WEI       SHAOW6@UCI.EDU  MCSB    G6      GR</t>
+  </si>
+  <si>
+    <t>19919996        SILKWOOD, KAI   KSILKWOO@UCI.EDU        MCSB    G6      GR</t>
+  </si>
+  <si>
+    <t>12442257        TAN, PEI        PEIT3@UCI.EDU   MCSB    G5      GR</t>
+  </si>
+  <si>
+    <t>63083899        TRAN, NHAT THANH VAN    NHATTT@UCI.EDU  MATH    G6      GR</t>
+  </si>
+  <si>
+    <t>92807178        WANG, TIANHONG  TIANHOW1@UCI.EDU        MATH+BIO SCI    SR      GR</t>
+  </si>
+  <si>
+    <t>22924311        WEI, SIYANG     SIYANGW2@UCI.EDU        MATH    G6      GR</t>
+  </si>
+  <si>
+    <t>39367708        ZAMORA, ANTHONY ZAMORAA3@UCI.EDU        MATH    G6      GR</t>
+  </si>
+  <si>
+    <t>Peijin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -174,6 +231,12 @@
       <name val="Times"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -196,11 +259,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -519,7 +583,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,23 +593,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="E2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -554,211 +624,245 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="E5" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C19" s="3"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -782,5 +886,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add to student list M227C
</commit_message>
<xml_diff>
--- a/studentList_M227C.xlsx
+++ b/studentList_M227C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/int/makeSmallGroups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2318B72-2BA8-CD43-9CB3-97749A633075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E107CD-D5EC-5448-B4DC-7E43AAA4085E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37240" yWindow="3080" windowWidth="22140" windowHeight="21380" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Chaorong</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Peijin</t>
+  </si>
+  <si>
+    <t>Kojo</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,6 +872,9 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
       <c r="C20" s="3"/>
       <c r="E20" s="1"/>
       <c r="F20" s="3"/>

</xml_diff>

<commit_message>
added missing student name
</commit_message>
<xml_diff>
--- a/studentList_M227C.xlsx
+++ b/studentList_M227C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E107CD-D5EC-5448-B4DC-7E43AAA4085E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32A1EA4-9695-0A40-8BAE-BE57808CFD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Chaorong</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Kojo</t>
+  </si>
+  <si>
+    <t>Tianhong</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,6 +886,9 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
       <c r="C21" s="3"/>
       <c r="E21" s="1"/>
       <c r="F21" s="3"/>

</xml_diff>

<commit_message>
virtual env for old version of drawSvg
</commit_message>
<xml_diff>
--- a/studentList_M227C.xlsx
+++ b/studentList_M227C.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32A1EA4-9695-0A40-8BAE-BE57808CFD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B712218-4CF7-144A-89A5-A942C279EDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
   </bookViews>
@@ -34,181 +34,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
-  <si>
-    <t>Chaorong</t>
-  </si>
-  <si>
-    <t>Gabby</t>
-  </si>
-  <si>
-    <t>Andres</t>
-  </si>
-  <si>
-    <t>Lulu</t>
-  </si>
-  <si>
-    <t>Thao</t>
-  </si>
-  <si>
-    <t>Negin</t>
-  </si>
-  <si>
-    <t>Wei</t>
-  </si>
-  <si>
-    <t>Kai</t>
-  </si>
-  <si>
-    <t>Pei</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Students</t>
   </si>
   <si>
-    <t>CHEN, CHAORONG</t>
-  </si>
-  <si>
-    <t>DE ROBLES, GABRIELA</t>
-  </si>
-  <si>
-    <t>ELDEEN, SARAH</t>
-  </si>
-  <si>
-    <t>GUERRERO RAMIREZ, ANDRES FELIPE</t>
-  </si>
-  <si>
-    <t>HE, YIYUN</t>
-  </si>
-  <si>
-    <t>IYER, VIGNESH HARIHARAN</t>
-  </si>
-  <si>
-    <t>LAI, LULU</t>
-  </si>
-  <si>
-    <t>NGUYEN, THI THU THAO</t>
-  </si>
-  <si>
-    <t>OLARANONT, NONTHAKORN</t>
-  </si>
-  <si>
-    <t>RAHIMZADEH, NEGIN</t>
-  </si>
-  <si>
-    <t>RUAN, YIBIAO</t>
-  </si>
-  <si>
-    <t>SHAO, WEI</t>
-  </si>
-  <si>
-    <t>SILKWOOD, KAI</t>
-  </si>
-  <si>
-    <t>TAN, PEI</t>
-  </si>
-  <si>
-    <t>TRAN, NHAT THANH VAN</t>
-  </si>
-  <si>
-    <t>WEI, SIYANG</t>
-  </si>
-  <si>
-    <t>ZAMORA, ANTHONY</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Yiyun</t>
-  </si>
-  <si>
-    <t>Vignesh</t>
-  </si>
-  <si>
-    <t>Nonthakorn</t>
-  </si>
-  <si>
-    <t>Yibiao</t>
-  </si>
-  <si>
-    <t>Nhat Thanh Van</t>
-  </si>
-  <si>
-    <t>Siyang</t>
-  </si>
-  <si>
-    <t>Anthony</t>
-  </si>
-  <si>
-    <t>85121744        CHEN, CHAORONG  CHAORONC@UCI.EDU        MCSB    G6      GR</t>
-  </si>
-  <si>
-    <t>15841424        DE ROBLES, GABRIELA     GDEROBLE@UCI.EDU        MCSB    G5      GR</t>
-  </si>
-  <si>
-    <t>21244597        ELDEEN, SARAH   SELDEEN@UCI.EDU MCSB    G6      GR</t>
-  </si>
-  <si>
-    <t>84549672        GAO, PEIJUN     PEIJUNG@UCI.EDU MATH    JR      GR</t>
-  </si>
-  <si>
-    <t>25167480        GUERRERO RAMIREZ, ANDRES FELIPE AFGUERRE@UCI.EDU        MCSB    G6      GR</t>
-  </si>
-  <si>
-    <t>18249792        IYER, VIGNESH HARIHARAN VHIYER@UCI.EDU  MATH    G5      GR</t>
-  </si>
-  <si>
-    <t>49527062        LAI, LULU       LLAI7@UCI.EDU   MCSB    G6      GR</t>
-  </si>
-  <si>
-    <t>84409046        NGUYEN, THI THU THAO    THAOTN18@UCI.EDU        MCSB    G6      GR</t>
-  </si>
-  <si>
-    <t>61007128        OLARANONT, NONTHAKORN   NOLARANO@UCI.EDU        MATH    G6      GR</t>
-  </si>
-  <si>
-    <t>41761116        RAHIMZADEH, NEGIN       NRAHIMZA@UCI.EDU        MCSB    G6      GR</t>
-  </si>
-  <si>
-    <t>13522870        RUAN, YIBIAO    YIBIAOR@UCI.EDU MATH    G5      GR</t>
-  </si>
-  <si>
-    <t>90727596        SHAO, WEI       SHAOW6@UCI.EDU  MCSB    G6      GR</t>
-  </si>
-  <si>
-    <t>19919996        SILKWOOD, KAI   KSILKWOO@UCI.EDU        MCSB    G6      GR</t>
-  </si>
-  <si>
-    <t>12442257        TAN, PEI        PEIT3@UCI.EDU   MCSB    G5      GR</t>
-  </si>
-  <si>
-    <t>63083899        TRAN, NHAT THANH VAN    NHATTT@UCI.EDU  MATH    G6      GR</t>
-  </si>
-  <si>
-    <t>92807178        WANG, TIANHONG  TIANHOW1@UCI.EDU        MATH+BIO SCI    SR      GR</t>
-  </si>
-  <si>
-    <t>22924311        WEI, SIYANG     SIYANGW2@UCI.EDU        MATH    G6      GR</t>
-  </si>
-  <si>
-    <t>39367708        ZAMORA, ANTHONY ZAMORAA3@UCI.EDU        MATH    G6      GR</t>
-  </si>
-  <si>
-    <t>Peijin</t>
-  </si>
-  <si>
-    <t>Kojo</t>
-  </si>
-  <si>
-    <t>Tianhong</t>
+    <t>Manuel</t>
+  </si>
+  <si>
+    <t>Brady</t>
+  </si>
+  <si>
+    <t>Yeon</t>
+  </si>
+  <si>
+    <t>Lorenzo</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Yuna</t>
+  </si>
+  <si>
+    <t>Jaewook</t>
+  </si>
+  <si>
+    <t>Joohu</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Ian</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Nima</t>
+  </si>
+  <si>
+    <t>Sai</t>
+  </si>
+  <si>
+    <t>Yonghan (Addie)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -243,6 +120,11 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -265,12 +147,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -586,298 +469,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126A2D9E-F695-4645-8524-97D12A4669B8}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="3.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>3</v>
+      </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="E6" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="E7" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="E8" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="E10" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="E11" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="E12" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="E13" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="E14" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="E15" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
+    <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="E16" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="E16" s="4"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="E17" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="E17" s="4"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>25</v>
-      </c>
+    <row r="18" spans="2:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="E18" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="E18" s="4"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>26</v>
-      </c>
+    <row r="19" spans="2:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="E19" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>54</v>
-      </c>
+    <row r="20" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C20" s="3"/>
       <c r="E20" s="1"/>
       <c r="F20" s="3"/>
@@ -885,10 +683,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>55</v>
-      </c>
+    <row r="21" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C21" s="3"/>
       <c r="E21" s="1"/>
       <c r="F21" s="3"/>

</xml_diff>

<commit_message>
modify for spring 2023
</commit_message>
<xml_diff>
--- a/studentList_M227C.xlsx
+++ b/studentList_M227C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B712218-4CF7-144A-89A5-A942C279EDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF535FDE-8953-0A44-AA58-859163F1BCA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>Sai</t>
   </si>
   <si>
-    <t>Yonghan (Addie)</t>
+    <t>Addie</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update for 2023 classroom
</commit_message>
<xml_diff>
--- a/studentList_M227C.xlsx
+++ b/studentList_M227C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/git/pub/makeSmallGroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B712218-4CF7-144A-89A5-A942C279EDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68D24DF-FACF-8C45-B125-74A82BA25F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="27520" windowHeight="17500" xr2:uid="{39EDD00D-2660-A84E-A731-C58DB0297BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Students</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Jaewook</t>
   </si>
   <si>
-    <t>Joohu</t>
-  </si>
-  <si>
     <t>Cameron</t>
   </si>
   <si>
@@ -78,7 +75,7 @@
     <t>Sai</t>
   </si>
   <si>
-    <t>Yonghan (Addie)</t>
+    <t>Addie</t>
   </si>
 </sst>
 </file>
@@ -472,7 +469,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A9" sqref="A9:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,9 +625,6 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="E15" s="4"/>

</xml_diff>